<commit_message>
Updated U6 LCSC part number
U6 TI SN74LVC1G3157DCKR, LCSC Part # C38663 is EOL in the parts library. Changed to equivalent Nexperia 74LVC1G3157GW, LCSC Part # C265126.
</commit_message>
<xml_diff>
--- a/JLCSMT_CCRv25su_BOM.xlsx
+++ b/JLCSMT_CCRv25su_BOM.xlsx
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>U6</t>
-  </si>
-  <si>
-    <t>C38663</t>
   </si>
   <si>
     <t>C77131</t>
@@ -331,9 +328,6 @@
     <t>F1, F2, F3</t>
   </si>
   <si>
-    <t>SN74LVC1G3157SC70-6</t>
-  </si>
-  <si>
     <t>SS54</t>
   </si>
   <si>
@@ -458,6 +452,12 @@
   </si>
   <si>
     <t>D1, D3, D4</t>
+  </si>
+  <si>
+    <t>C265126</t>
+  </si>
+  <si>
+    <t>74LVC1G3157GW</t>
   </si>
 </sst>
 </file>
@@ -848,8 +848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -862,61 +862,61 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="42.75">
       <c r="A3" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -924,10 +924,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>2</v>
@@ -935,50 +935,50 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="C8" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -986,66 +986,66 @@
         <v>10</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="42.75">
       <c r="A10" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="C11" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="C12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="C13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>0</v>
@@ -1053,13 +1053,13 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>1</v>
@@ -1067,30 +1067,30 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="C15" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="C16" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1098,41 +1098,41 @@
         <v>100</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>69</v>
-      </c>
       <c r="C18" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1140,41 +1140,41 @@
         <v>120</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="C22" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1182,13 +1182,13 @@
         <v>680</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1196,272 +1196,272 @@
         <v>820</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E25" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E29" s="5"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="C30" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="C31" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="C32" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="C34" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>88</v>
-      </c>
       <c r="C35" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="4" t="s">
-        <v>89</v>
+        <v>131</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>5</v>
+        <v>130</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E39" s="5"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>